<commit_message>
added MD5 Hash column
</commit_message>
<xml_diff>
--- a/ArchiveDetails.xlsx
+++ b/ArchiveDetails.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Overview" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Archives!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Archives!$A$1:$G$37</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Archive Name</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>MD5 Hash</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,9 +405,10 @@
     <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,9 +427,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:G37"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>